<commit_message>
Multiple Updates: Make prey type UNID 1st row, allow blank preytype for non-prey, add aged adult pawsize, add lobster prey class
</commit_message>
<xml_diff>
--- a/helperfiles/Pawsz.xlsx
+++ b/helperfiles/Pawsz.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tim Tinker\OneDrive\Documents\Nhydra\Projects\SOFA2\SOFA\data\WASH_2010_2020_SA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/26362cec7e0913ab/Documents/Nhydra/Projects/SOFA2/SOFA/helperfiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B23B6093-2D70-4E3B-B6FA-5A19D7B6DC95}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="12" documentId="13_ncr:1_{B23B6093-2D70-4E3B-B6FA-5A19D7B6DC95}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{55D6347D-AA9F-4031-93C0-4F61A913C15D}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="27930" windowHeight="15165" xr2:uid="{CAFB1425-1709-401D-9C9C-CCBF2AAB893B}"/>
+    <workbookView xWindow="30495" yWindow="1170" windowWidth="24150" windowHeight="14760" xr2:uid="{CAFB1425-1709-401D-9C9C-CCBF2AAB893B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="10">
   <si>
     <t>Sex</t>
   </si>
@@ -61,6 +61,9 @@
   </si>
   <si>
     <t>sa</t>
+  </si>
+  <si>
+    <t>aa</t>
   </si>
 </sst>
 </file>
@@ -422,10 +425,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52D15186-7DA0-45A6-9358-4F0D59B3A8B9}">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection sqref="A1:C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -479,21 +482,21 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C5">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C6">
-        <v>42</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -501,10 +504,10 @@
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C7">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -512,10 +515,10 @@
         <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C8">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -523,34 +526,32 @@
         <v>4</v>
       </c>
       <c r="B9" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C9">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B10" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C10">
-        <f>(C2+C6)/2</f>
-        <v>41</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B11" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C11">
-        <f t="shared" ref="C11:C13" si="0">(C3+C7)/2</f>
-        <v>44.5</v>
+        <v>48</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -558,11 +559,11 @@
         <v>5</v>
       </c>
       <c r="B12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C12">
-        <f t="shared" si="0"/>
-        <v>48</v>
+        <f>(C2+C7)/2</f>
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -570,10 +571,46 @@
         <v>5</v>
       </c>
       <c r="B13" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C13">
-        <f t="shared" si="0"/>
+        <f>(C3+C8)/2</f>
+        <v>44.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14">
+        <f>(C4+C9)/2</f>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15">
+        <f>(C5+C10)/2</f>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16">
+        <f>(C6+C11)/2</f>
         <v>47</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fix pawsize file typo
</commit_message>
<xml_diff>
--- a/helperfiles/Pawsz.xlsx
+++ b/helperfiles/Pawsz.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/26362cec7e0913ab/Documents/Nhydra/Projects/SOFA2/SOFA/helperfiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="12" documentId="13_ncr:1_{B23B6093-2D70-4E3B-B6FA-5A19D7B6DC95}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{55D6347D-AA9F-4031-93C0-4F61A913C15D}"/>
+  <xr:revisionPtr revIDLastSave="13" documentId="13_ncr:1_{B23B6093-2D70-4E3B-B6FA-5A19D7B6DC95}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{31BCBF29-D70F-4644-977A-4EFE93B50F17}"/>
   <bookViews>
-    <workbookView xWindow="30495" yWindow="1170" windowWidth="24150" windowHeight="14760" xr2:uid="{CAFB1425-1709-401D-9C9C-CCBF2AAB893B}"/>
+    <workbookView xWindow="30630" yWindow="840" windowWidth="24150" windowHeight="14760" xr2:uid="{CAFB1425-1709-401D-9C9C-CCBF2AAB893B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -428,7 +428,7 @@
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C16"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -537,7 +537,7 @@
         <v>4</v>
       </c>
       <c r="B10" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C10">
         <v>49</v>

</xml_diff>

<commit_message>
Version 3.1 very minor updates
</commit_message>
<xml_diff>
--- a/helperfiles/Pawsz.xlsx
+++ b/helperfiles/Pawsz.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/26362cec7e0913ab/Documents/Nhydra/Projects/SOFA2/SOFA/helperfiles/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nhydra-my.sharepoint.com/personal/ttinker_nhydra-eco_com/Documents/SOFA2/SOFA/helperfiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="13" documentId="13_ncr:1_{B23B6093-2D70-4E3B-B6FA-5A19D7B6DC95}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{31BCBF29-D70F-4644-977A-4EFE93B50F17}"/>
+  <xr:revisionPtr revIDLastSave="18" documentId="13_ncr:1_{B23B6093-2D70-4E3B-B6FA-5A19D7B6DC95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C57B625C-BA18-41C6-94E5-D8014A5DDF14}"/>
   <bookViews>
-    <workbookView xWindow="30630" yWindow="840" windowWidth="24150" windowHeight="14760" xr2:uid="{CAFB1425-1709-401D-9C9C-CCBF2AAB893B}"/>
+    <workbookView xWindow="2445" yWindow="390" windowWidth="46650" windowHeight="20175" xr2:uid="{CAFB1425-1709-401D-9C9C-CCBF2AAB893B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -108,9 +108,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -129,9 +132,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -169,7 +172,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -275,7 +278,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -417,7 +420,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -425,15 +428,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52D15186-7DA0-45A6-9358-4F0D59B3A8B9}">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="E4" sqref="E4:H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -444,7 +447,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -455,7 +458,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -466,7 +469,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -476,8 +479,10 @@
       <c r="C4">
         <v>47</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -488,7 +493,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -499,7 +504,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -510,7 +515,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -521,7 +526,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -532,7 +537,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -543,7 +548,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>4</v>
       </c>
@@ -554,7 +559,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>5</v>
       </c>
@@ -566,7 +571,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>5</v>
       </c>
@@ -578,7 +583,7 @@
         <v>44.5</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>5</v>
       </c>
@@ -590,7 +595,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>5</v>
       </c>
@@ -602,7 +607,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>5</v>
       </c>

</xml_diff>